<commit_message>
96.5 acc for 10 classes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asadi\OneDrive\Desktop\UofT\Year3\Winter\ECE324\PodcastClassifier\ece324PodcastClassifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD7AEF47-CE9F-4302-864B-263D86087FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66757FA-FFD6-4B5F-ABA1-83E1457C6B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{907972F9-E2E4-4A1F-888F-C9F6B11BDE33}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>num classes</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>2 bears one cave, the views, andrew schulz, impaulsive, joe rogan</t>
+  </si>
+  <si>
+    <t>2 bears one cave, the views, andrew schulz, impaulsive, joe rogan, h3h3, jenna and julien, lex fridman, off topic, optic podcast</t>
   </si>
 </sst>
 </file>
@@ -402,16 +405,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051AA7FA-A4F4-4788-BB27-AC8AC1A53AFF}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.54296875" customWidth="1"/>
-    <col min="2" max="2" width="72.54296875" customWidth="1"/>
+    <col min="2" max="2" width="104.7265625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -448,6 +451,17 @@
         <v>98.4</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>96.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20 classes 95 acc
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asadi\OneDrive\Desktop\UofT\Year3\Winter\ECE324\PodcastClassifier\ece324PodcastClassifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66757FA-FFD6-4B5F-ABA1-83E1457C6B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412B2007-56E1-4534-8881-CABF25538546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{907972F9-E2E4-4A1F-888F-C9F6B11BDE33}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>num classes</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>2 bears one cave, the views, andrew schulz, impaulsive, joe rogan, h3h3, jenna and julien, lex fridman, off topic, optic podcast</t>
+  </si>
+  <si>
+    <t>first 20 in data folder</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051AA7FA-A4F4-4788-BB27-AC8AC1A53AFF}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -453,13 +456,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4">
         <v>96.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>96.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
95% on all classes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asadi\OneDrive\Desktop\UofT\Year3\Winter\ECE324\PodcastClassifier\ece324PodcastClassifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412B2007-56E1-4534-8881-CABF25538546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2D7340-739A-4EAE-8491-190F2D5C138A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{907972F9-E2E4-4A1F-888F-C9F6B11BDE33}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>num classes</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>first 20 in data folder</t>
+  </si>
+  <si>
+    <t>first 30 in data folder</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051AA7FA-A4F4-4788-BB27-AC8AC1A53AFF}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -476,6 +482,25 @@
         <v>96.2</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>95.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>